<commit_message>
updates to QMe documents
</commit_message>
<xml_diff>
--- a/documents/QMe_UserStories.xlsx
+++ b/documents/QMe_UserStories.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="190">
   <si>
     <t>Project</t>
   </si>
@@ -371,6 +371,15 @@
     <t>FOREIGN KEY CATEGORY</t>
   </si>
   <si>
+    <t>USER_CATEGORY_LIKES</t>
+  </si>
+  <si>
+    <t>Primary Key/FOREIGN KEY USER</t>
+  </si>
+  <si>
+    <t>Primary Key/FOREIGN KEY CATEGORY</t>
+  </si>
+  <si>
     <t>QUESTION</t>
   </si>
   <si>
@@ -428,10 +437,13 @@
     <t>ANSWER_REF_MEDIA_ID</t>
   </si>
   <si>
-    <t>REF_MEDIA_TYPE</t>
-  </si>
-  <si>
-    <t>VARCHAR(50)</t>
+    <t>MEDIA_TYPE_ID</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY MEDIA_TYPE</t>
+  </si>
+  <si>
+    <t>REF_MEDIA_MIME</t>
   </si>
   <si>
     <t>REF_MEDIA</t>
@@ -470,7 +482,7 @@
     <t>FOREIGN KEY ANSWER_OPTION</t>
   </si>
   <si>
-    <t>OPTION_MEDIA_TYPE</t>
+    <t>OPTION_MEDIA_MIME</t>
   </si>
   <si>
     <t>OPTION_MEDIA</t>
@@ -570,6 +582,12 @@
   </si>
   <si>
     <t>Primary Key /  FOREIGN KEY QUIZ</t>
+  </si>
+  <si>
+    <t>MEDIA_TYPE</t>
+  </si>
+  <si>
+    <t>MEDIA_TYPE_DESC</t>
   </si>
 </sst>
 </file>
@@ -655,7 +673,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -888,13 +906,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1039,8 +1072,17 @@
     <xf numFmtId="1" fontId="1" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
@@ -1280,9 +1322,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>99099</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>138586</xdr:rowOff>
+      <xdr:colOff>374191</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>21118</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1299,8 +1341,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="-73351"/>
-          <a:ext cx="7592100" cy="8647587"/>
+          <a:off x="-1" y="0"/>
+          <a:ext cx="7867193" cy="9501669"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2657,10 +2699,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="A3:A11"/>
     <mergeCell ref="B3:F11"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
@@ -3753,7 +3795,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -4107,18 +4149,18 @@
         <v>117</v>
       </c>
       <c r="C29" t="s" s="38">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E29" t="s" s="39">
-        <v>82</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" ht="16" customHeight="1">
-      <c r="A30" s="46"/>
-      <c r="B30" s="46"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
       <c r="C30" t="s" s="38">
         <v>108</v>
       </c>
@@ -4126,202 +4168,202 @@
         <v>90</v>
       </c>
       <c r="E30" t="s" s="39">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" ht="16" customHeight="1">
-      <c r="A31" s="46"/>
-      <c r="B31" s="46"/>
-      <c r="C31" t="s" s="38">
-        <v>119</v>
-      </c>
-      <c r="D31" t="s" s="38">
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="49"/>
+    </row>
+    <row r="32" ht="16" customHeight="1">
+      <c r="A32" s="43"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="45"/>
+    </row>
+    <row r="33" ht="16" customHeight="1">
+      <c r="A33" s="36">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s" s="37">
         <v>120</v>
       </c>
-      <c r="E31" s="42"/>
-    </row>
-    <row r="32" ht="16" customHeight="1">
-      <c r="A32" s="46"/>
-      <c r="B32" s="46"/>
-      <c r="C32" t="s" s="38">
+      <c r="C33" t="s" s="38">
         <v>121</v>
-      </c>
-      <c r="D32" t="s" s="38">
-        <v>122</v>
-      </c>
-      <c r="E32" s="42"/>
-    </row>
-    <row r="33" ht="16" customHeight="1">
-      <c r="A33" s="46"/>
-      <c r="B33" s="46"/>
-      <c r="C33" t="s" s="38">
-        <v>123</v>
       </c>
       <c r="D33" t="s" s="38">
         <v>90</v>
       </c>
-      <c r="E33" s="42"/>
+      <c r="E33" t="s" s="39">
+        <v>82</v>
+      </c>
     </row>
     <row r="34" ht="16" customHeight="1">
       <c r="A34" s="46"/>
       <c r="B34" s="46"/>
       <c r="C34" t="s" s="38">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="D34" t="s" s="38">
-        <v>101</v>
-      </c>
-      <c r="E34" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E34" t="s" s="39">
+        <v>116</v>
+      </c>
     </row>
     <row r="35" ht="16" customHeight="1">
       <c r="A35" s="46"/>
       <c r="B35" s="46"/>
       <c r="C35" t="s" s="38">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D35" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E35" t="s" s="39">
-        <v>105</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="E35" s="42"/>
     </row>
     <row r="36" ht="16" customHeight="1">
       <c r="A36" s="46"/>
       <c r="B36" s="46"/>
       <c r="C36" t="s" s="38">
+        <v>124</v>
+      </c>
+      <c r="D36" t="s" s="38">
+        <v>125</v>
+      </c>
+      <c r="E36" s="42"/>
+    </row>
+    <row r="37" ht="16" customHeight="1">
+      <c r="A37" s="46"/>
+      <c r="B37" s="46"/>
+      <c r="C37" t="s" s="38">
         <v>126</v>
-      </c>
-      <c r="D36" t="s" s="38">
-        <v>101</v>
-      </c>
-      <c r="E36" s="42"/>
-    </row>
-    <row r="37" ht="16" customHeight="1">
-      <c r="A37" s="47"/>
-      <c r="B37" s="47"/>
-      <c r="C37" t="s" s="38">
-        <v>127</v>
       </c>
       <c r="D37" t="s" s="38">
         <v>90</v>
       </c>
-      <c r="E37" t="s" s="39">
-        <v>105</v>
-      </c>
+      <c r="E37" s="42"/>
     </row>
     <row r="38" ht="16" customHeight="1">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="45"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="46"/>
+      <c r="C38" t="s" s="38">
+        <v>127</v>
+      </c>
+      <c r="D38" t="s" s="38">
+        <v>101</v>
+      </c>
+      <c r="E38" s="42"/>
     </row>
     <row r="39" ht="16" customHeight="1">
-      <c r="A39" s="36">
-        <v>7</v>
-      </c>
-      <c r="B39" t="s" s="37">
+      <c r="A39" s="46"/>
+      <c r="B39" s="46"/>
+      <c r="C39" t="s" s="38">
         <v>128</v>
-      </c>
-      <c r="C39" t="s" s="38">
-        <v>118</v>
       </c>
       <c r="D39" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E39" t="s" s="39">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" ht="16" customHeight="1">
       <c r="A40" s="46"/>
       <c r="B40" s="46"/>
       <c r="C40" t="s" s="38">
+        <v>129</v>
+      </c>
+      <c r="D40" t="s" s="38">
+        <v>101</v>
+      </c>
+      <c r="E40" s="42"/>
+    </row>
+    <row r="41" ht="16" customHeight="1">
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
+      <c r="C41" t="s" s="38">
+        <v>130</v>
+      </c>
+      <c r="D41" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E41" t="s" s="39">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" ht="16" customHeight="1">
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="45"/>
+    </row>
+    <row r="43" ht="16" customHeight="1">
+      <c r="A43" s="36">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s" s="37">
+        <v>131</v>
+      </c>
+      <c r="C43" t="s" s="38">
+        <v>121</v>
+      </c>
+      <c r="D43" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E43" t="s" s="39">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" ht="16" customHeight="1">
+      <c r="A44" s="46"/>
+      <c r="B44" s="46"/>
+      <c r="C44" t="s" s="38">
         <v>108</v>
       </c>
-      <c r="D40" t="s" s="38">
+      <c r="D44" t="s" s="38">
         <v>90</v>
       </c>
-      <c r="E40" t="s" s="39">
+      <c r="E44" t="s" s="39">
         <v>116</v>
       </c>
     </row>
-    <row r="41" ht="16" customHeight="1">
-      <c r="A41" s="46"/>
-      <c r="B41" s="46"/>
-      <c r="C41" t="s" s="38">
-        <v>128</v>
-      </c>
-      <c r="D41" t="s" s="38">
+    <row r="45" ht="16" customHeight="1">
+      <c r="A45" s="46"/>
+      <c r="B45" s="46"/>
+      <c r="C45" t="s" s="38">
+        <v>131</v>
+      </c>
+      <c r="D45" t="s" s="38">
         <v>81</v>
       </c>
-      <c r="E41" s="42"/>
-    </row>
-    <row r="42" ht="16" customHeight="1">
-      <c r="A42" s="46"/>
-      <c r="B42" s="46"/>
-      <c r="C42" t="s" s="38">
-        <v>130</v>
-      </c>
-      <c r="D42" t="s" s="38">
-        <v>81</v>
-      </c>
-      <c r="E42" s="42"/>
-    </row>
-    <row r="43" ht="16" customHeight="1">
-      <c r="A43" s="47"/>
-      <c r="B43" s="47"/>
-      <c r="C43" t="s" s="38">
-        <v>131</v>
-      </c>
-      <c r="D43" t="s" s="38">
-        <v>81</v>
-      </c>
-      <c r="E43" s="42"/>
-    </row>
-    <row r="44" ht="16" customHeight="1">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="45"/>
-    </row>
-    <row r="45" ht="16" customHeight="1">
-      <c r="A45" s="36">
-        <v>8</v>
-      </c>
-      <c r="B45" t="s" s="37">
-        <v>132</v>
-      </c>
-      <c r="C45" t="s" s="38">
-        <v>89</v>
-      </c>
-      <c r="D45" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E45" t="s" s="39">
-        <v>133</v>
-      </c>
+      <c r="E45" s="42"/>
     </row>
     <row r="46" ht="16" customHeight="1">
       <c r="A46" s="46"/>
       <c r="B46" s="46"/>
       <c r="C46" t="s" s="38">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="D46" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E46" t="s" s="39">
-        <v>129</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="E46" s="42"/>
     </row>
     <row r="47" ht="16" customHeight="1">
       <c r="A47" s="47"/>
       <c r="B47" s="47"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
+      <c r="C47" t="s" s="38">
+        <v>134</v>
+      </c>
+      <c r="D47" t="s" s="38">
+        <v>81</v>
+      </c>
       <c r="E47" s="42"/>
     </row>
     <row r="48" ht="16" customHeight="1">
@@ -4336,98 +4378,96 @@
         <v>9</v>
       </c>
       <c r="B49" t="s" s="37">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C49" t="s" s="38">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="D49" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E49" t="s" s="39">
-        <v>82</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" ht="16" customHeight="1">
       <c r="A50" s="46"/>
       <c r="B50" s="46"/>
       <c r="C50" t="s" s="38">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D50" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E50" t="s" s="39">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" ht="16" customHeight="1">
-      <c r="A51" s="46"/>
-      <c r="B51" s="46"/>
-      <c r="C51" t="s" s="38">
-        <v>136</v>
-      </c>
-      <c r="D51" t="s" s="38">
+      <c r="A51" s="47"/>
+      <c r="B51" s="47"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="42"/>
+    </row>
+    <row r="52" ht="16" customHeight="1">
+      <c r="A52" s="43"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="45"/>
+    </row>
+    <row r="53" ht="16" customHeight="1">
+      <c r="A53" s="36">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s" s="37">
         <v>137</v>
       </c>
-      <c r="E51" s="42"/>
-    </row>
-    <row r="52" ht="16" customHeight="1">
-      <c r="A52" s="47"/>
-      <c r="B52" s="47"/>
-      <c r="C52" t="s" s="38">
+      <c r="C53" t="s" s="38">
         <v>138</v>
       </c>
-      <c r="D52" t="s" s="38">
-        <v>139</v>
-      </c>
-      <c r="E52" s="42"/>
-    </row>
-    <row r="53" ht="16" customHeight="1">
-      <c r="A53" s="43"/>
-      <c r="B53" s="43"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="45"/>
+      <c r="D53" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E53" t="s" s="39">
+        <v>82</v>
+      </c>
     </row>
     <row r="54" ht="16" customHeight="1">
-      <c r="A54" s="36">
-        <v>10</v>
-      </c>
-      <c r="B54" t="s" s="37">
-        <v>140</v>
-      </c>
+      <c r="A54" s="46"/>
+      <c r="B54" s="46"/>
       <c r="C54" t="s" s="38">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="D54" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E54" t="s" s="39">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" ht="16" customHeight="1">
       <c r="A55" s="46"/>
       <c r="B55" s="46"/>
       <c r="C55" t="s" s="38">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="D55" t="s" s="38">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E55" t="s" s="39">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" ht="16" customHeight="1">
-      <c r="A56" s="46"/>
-      <c r="B56" s="46"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="51"/>
       <c r="C56" t="s" s="38">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D56" t="s" s="38">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E56" s="42"/>
     </row>
@@ -4435,14 +4475,12 @@
       <c r="A57" s="47"/>
       <c r="B57" s="47"/>
       <c r="C57" t="s" s="38">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D57" t="s" s="38">
-        <v>145</v>
-      </c>
-      <c r="E57" t="s" s="39">
-        <v>146</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="E57" s="42"/>
     </row>
     <row r="58" ht="16" customHeight="1">
       <c r="A58" s="43"/>
@@ -4456,10 +4494,10 @@
         <v>11</v>
       </c>
       <c r="B59" t="s" s="37">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C59" t="s" s="38">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D59" t="s" s="38">
         <v>90</v>
@@ -4472,23 +4510,23 @@
       <c r="A60" s="46"/>
       <c r="B60" s="46"/>
       <c r="C60" t="s" s="38">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="D60" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E60" t="s" s="39">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" ht="16" customHeight="1">
       <c r="A61" s="46"/>
       <c r="B61" s="46"/>
       <c r="C61" t="s" s="38">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D61" t="s" s="38">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E61" s="42"/>
     </row>
@@ -4496,12 +4534,14 @@
       <c r="A62" s="47"/>
       <c r="B62" s="47"/>
       <c r="C62" t="s" s="38">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D62" t="s" s="38">
-        <v>139</v>
-      </c>
-      <c r="E62" s="42"/>
+        <v>149</v>
+      </c>
+      <c r="E62" t="s" s="39">
+        <v>150</v>
+      </c>
     </row>
     <row r="63" ht="16" customHeight="1">
       <c r="A63" s="43"/>
@@ -4515,10 +4555,10 @@
         <v>12</v>
       </c>
       <c r="B64" t="s" s="37">
+        <v>151</v>
+      </c>
+      <c r="C64" t="s" s="38">
         <v>152</v>
-      </c>
-      <c r="C64" t="s" s="38">
-        <v>153</v>
       </c>
       <c r="D64" t="s" s="38">
         <v>90</v>
@@ -4531,78 +4571,82 @@
       <c r="A65" s="46"/>
       <c r="B65" s="46"/>
       <c r="C65" t="s" s="38">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D65" t="s" s="38">
-        <v>155</v>
-      </c>
-      <c r="E65" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E65" t="s" s="39">
+        <v>153</v>
+      </c>
     </row>
     <row r="66" ht="16" customHeight="1">
       <c r="A66" s="46"/>
       <c r="B66" s="46"/>
       <c r="C66" t="s" s="38">
+        <v>139</v>
+      </c>
+      <c r="D66" t="s" s="38">
+        <v>81</v>
+      </c>
+      <c r="E66" t="s" s="39">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" ht="16" customHeight="1">
+      <c r="A67" s="31"/>
+      <c r="B67" s="51"/>
+      <c r="C67" t="s" s="38">
+        <v>154</v>
+      </c>
+      <c r="D67" t="s" s="38">
+        <v>110</v>
+      </c>
+      <c r="E67" s="42"/>
+    </row>
+    <row r="68" ht="16" customHeight="1">
+      <c r="A68" s="47"/>
+      <c r="B68" s="47"/>
+      <c r="C68" t="s" s="38">
+        <v>155</v>
+      </c>
+      <c r="D68" t="s" s="38">
+        <v>143</v>
+      </c>
+      <c r="E68" s="42"/>
+    </row>
+    <row r="69" ht="16" customHeight="1">
+      <c r="A69" s="43"/>
+      <c r="B69" s="43"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="45"/>
+    </row>
+    <row r="70" ht="16" customHeight="1">
+      <c r="A70" s="36">
+        <v>13</v>
+      </c>
+      <c r="B70" t="s" s="37">
         <v>156</v>
       </c>
-      <c r="D66" t="s" s="38">
+      <c r="C70" t="s" s="38">
         <v>157</v>
       </c>
-      <c r="E66" s="42"/>
-    </row>
-    <row r="67" ht="16" customHeight="1">
-      <c r="A67" s="46"/>
-      <c r="B67" s="46"/>
-      <c r="C67" t="s" s="38">
-        <v>108</v>
-      </c>
-      <c r="D67" t="s" s="38">
+      <c r="D70" t="s" s="38">
         <v>90</v>
       </c>
-      <c r="E67" t="s" s="39">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="68" ht="16" customHeight="1">
-      <c r="A68" s="46"/>
-      <c r="B68" s="46"/>
-      <c r="C68" t="s" s="38">
-        <v>158</v>
-      </c>
-      <c r="D68" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E68" s="42"/>
-    </row>
-    <row r="69" ht="16" customHeight="1">
-      <c r="A69" s="46"/>
-      <c r="B69" s="46"/>
-      <c r="C69" t="s" s="38">
-        <v>159</v>
-      </c>
-      <c r="D69" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E69" s="42"/>
-    </row>
-    <row r="70" ht="16" customHeight="1">
-      <c r="A70" s="46"/>
-      <c r="B70" s="46"/>
-      <c r="C70" t="s" s="38">
-        <v>160</v>
-      </c>
-      <c r="D70" t="s" s="38">
-        <v>145</v>
-      </c>
-      <c r="E70" s="42"/>
+      <c r="E70" t="s" s="39">
+        <v>82</v>
+      </c>
     </row>
     <row r="71" ht="16" customHeight="1">
       <c r="A71" s="46"/>
       <c r="B71" s="46"/>
       <c r="C71" t="s" s="38">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D71" t="s" s="38">
-        <v>101</v>
+        <v>159</v>
       </c>
       <c r="E71" s="42"/>
     </row>
@@ -4610,259 +4654,257 @@
       <c r="A72" s="46"/>
       <c r="B72" s="46"/>
       <c r="C72" t="s" s="38">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D72" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E72" t="s" s="39">
-        <v>105</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="E72" s="42"/>
     </row>
     <row r="73" ht="16" customHeight="1">
       <c r="A73" s="46"/>
       <c r="B73" s="46"/>
       <c r="C73" t="s" s="38">
-        <v>163</v>
+        <v>108</v>
       </c>
       <c r="D73" t="s" s="38">
-        <v>101</v>
-      </c>
-      <c r="E73" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E73" t="s" s="39">
+        <v>116</v>
+      </c>
     </row>
     <row r="74" ht="16" customHeight="1">
       <c r="A74" s="46"/>
       <c r="B74" s="46"/>
       <c r="C74" t="s" s="38">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D74" t="s" s="38">
         <v>90</v>
       </c>
-      <c r="E74" t="s" s="39">
-        <v>105</v>
-      </c>
+      <c r="E74" s="42"/>
     </row>
     <row r="75" ht="16" customHeight="1">
-      <c r="A75" s="47"/>
-      <c r="B75" s="47"/>
-      <c r="C75" s="49"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="50"/>
+      <c r="A75" s="46"/>
+      <c r="B75" s="46"/>
+      <c r="C75" t="s" s="38">
+        <v>163</v>
+      </c>
+      <c r="D75" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E75" s="42"/>
     </row>
     <row r="76" ht="16" customHeight="1">
-      <c r="A76" s="43"/>
-      <c r="B76" s="43"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="45"/>
+      <c r="A76" s="46"/>
+      <c r="B76" s="46"/>
+      <c r="C76" t="s" s="38">
+        <v>164</v>
+      </c>
+      <c r="D76" t="s" s="38">
+        <v>149</v>
+      </c>
+      <c r="E76" s="42"/>
     </row>
     <row r="77" ht="16" customHeight="1">
-      <c r="A77" s="36">
-        <v>13</v>
-      </c>
-      <c r="B77" t="s" s="37">
+      <c r="A77" s="46"/>
+      <c r="B77" s="46"/>
+      <c r="C77" t="s" s="38">
         <v>165</v>
       </c>
-      <c r="C77" t="s" s="38">
-        <v>166</v>
-      </c>
       <c r="D77" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E77" t="s" s="39">
-        <v>82</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E77" s="42"/>
     </row>
     <row r="78" ht="16" customHeight="1">
       <c r="A78" s="46"/>
       <c r="B78" s="46"/>
       <c r="C78" t="s" s="38">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="D78" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E78" t="s" s="39">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" ht="16" customHeight="1">
+      <c r="A79" s="46"/>
+      <c r="B79" s="46"/>
+      <c r="C79" t="s" s="38">
         <v>167</v>
       </c>
-    </row>
-    <row r="79" ht="16" customHeight="1">
-      <c r="A79" s="47"/>
-      <c r="B79" s="47"/>
-      <c r="C79" t="s" s="38">
-        <v>118</v>
-      </c>
       <c r="D79" t="s" s="38">
+        <v>101</v>
+      </c>
+      <c r="E79" s="42"/>
+    </row>
+    <row r="80" ht="16" customHeight="1">
+      <c r="A80" s="46"/>
+      <c r="B80" s="46"/>
+      <c r="C80" t="s" s="38">
+        <v>168</v>
+      </c>
+      <c r="D80" t="s" s="38">
         <v>90</v>
       </c>
-      <c r="E79" t="s" s="39">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" ht="16" customHeight="1">
-      <c r="A80" s="43"/>
-      <c r="B80" s="43"/>
-      <c r="C80" s="44"/>
-      <c r="D80" s="44"/>
-      <c r="E80" s="45"/>
+      <c r="E80" t="s" s="39">
+        <v>105</v>
+      </c>
     </row>
     <row r="81" ht="16" customHeight="1">
-      <c r="A81" s="36">
+      <c r="A81" s="47"/>
+      <c r="B81" s="47"/>
+      <c r="C81" s="52"/>
+      <c r="D81" s="52"/>
+      <c r="E81" s="53"/>
+    </row>
+    <row r="82" ht="16" customHeight="1">
+      <c r="A82" s="43"/>
+      <c r="B82" s="43"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="45"/>
+    </row>
+    <row r="83" ht="16" customHeight="1">
+      <c r="A83" s="36">
         <v>14</v>
       </c>
-      <c r="B81" t="s" s="37">
-        <v>168</v>
-      </c>
-      <c r="C81" t="s" s="38">
+      <c r="B83" t="s" s="37">
         <v>169</v>
       </c>
-      <c r="D81" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E81" t="s" s="39">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="82" ht="16" customHeight="1">
-      <c r="A82" s="46"/>
-      <c r="B82" s="46"/>
-      <c r="C82" t="s" s="38">
-        <v>89</v>
-      </c>
-      <c r="D82" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E82" t="s" s="39">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="83" ht="16" customHeight="1">
-      <c r="A83" s="46"/>
-      <c r="B83" s="46"/>
       <c r="C83" t="s" s="38">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="D83" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E83" t="s" s="39">
-        <v>167</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" ht="16" customHeight="1">
       <c r="A84" s="46"/>
       <c r="B84" s="46"/>
       <c r="C84" t="s" s="38">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="D84" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E84" t="s" s="39">
-        <v>116</v>
+        <v>171</v>
       </c>
     </row>
     <row r="85" ht="16" customHeight="1">
-      <c r="A85" s="46"/>
-      <c r="B85" s="46"/>
+      <c r="A85" s="47"/>
+      <c r="B85" s="47"/>
       <c r="C85" t="s" s="38">
-        <v>170</v>
+        <v>121</v>
       </c>
       <c r="D85" t="s" s="38">
-        <v>101</v>
-      </c>
-      <c r="E85" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E85" t="s" s="39">
+        <v>146</v>
+      </c>
     </row>
     <row r="86" ht="16" customHeight="1">
-      <c r="A86" s="46"/>
-      <c r="B86" s="46"/>
-      <c r="C86" t="s" s="38">
-        <v>171</v>
-      </c>
-      <c r="D86" t="s" s="38">
-        <v>101</v>
-      </c>
-      <c r="E86" s="42"/>
+      <c r="A86" s="43"/>
+      <c r="B86" s="43"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="45"/>
     </row>
     <row r="87" ht="16" customHeight="1">
-      <c r="A87" s="46"/>
-      <c r="B87" s="46"/>
+      <c r="A87" s="36">
+        <v>15</v>
+      </c>
+      <c r="B87" t="s" s="37">
+        <v>172</v>
+      </c>
       <c r="C87" t="s" s="38">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D87" t="s" s="38">
-        <v>81</v>
-      </c>
-      <c r="E87" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E87" t="s" s="39">
+        <v>82</v>
+      </c>
     </row>
     <row r="88" ht="16" customHeight="1">
       <c r="A88" s="46"/>
       <c r="B88" s="46"/>
       <c r="C88" t="s" s="38">
-        <v>173</v>
+        <v>89</v>
       </c>
       <c r="D88" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E88" t="s" s="39">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="89" ht="16" customHeight="1">
+      <c r="A89" s="46"/>
+      <c r="B89" s="46"/>
+      <c r="C89" t="s" s="38">
+        <v>157</v>
+      </c>
+      <c r="D89" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E89" t="s" s="39">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" ht="16" customHeight="1">
+      <c r="A90" s="46"/>
+      <c r="B90" s="46"/>
+      <c r="C90" t="s" s="38">
+        <v>108</v>
+      </c>
+      <c r="D90" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E90" t="s" s="39">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" ht="16" customHeight="1">
+      <c r="A91" s="46"/>
+      <c r="B91" s="46"/>
+      <c r="C91" t="s" s="38">
         <v>174</v>
       </c>
-      <c r="E88" s="42"/>
-    </row>
-    <row r="89" ht="16" customHeight="1">
-      <c r="A89" s="47"/>
-      <c r="B89" s="47"/>
-      <c r="C89" t="s" s="38">
-        <v>175</v>
-      </c>
-      <c r="D89" t="s" s="38">
-        <v>145</v>
-      </c>
-      <c r="E89" s="42"/>
-    </row>
-    <row r="90" ht="16" customHeight="1">
-      <c r="A90" s="43"/>
-      <c r="B90" s="43"/>
-      <c r="C90" s="44"/>
-      <c r="D90" s="44"/>
-      <c r="E90" s="45"/>
-    </row>
-    <row r="91" ht="16" customHeight="1">
-      <c r="A91" s="36">
-        <v>15</v>
-      </c>
-      <c r="B91" t="s" s="37">
-        <v>176</v>
-      </c>
-      <c r="C91" t="s" s="38">
-        <v>89</v>
-      </c>
       <c r="D91" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E91" t="s" s="39">
-        <v>177</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E91" s="42"/>
     </row>
     <row r="92" ht="16" customHeight="1">
       <c r="A92" s="46"/>
       <c r="B92" s="46"/>
       <c r="C92" t="s" s="38">
-        <v>108</v>
+        <v>175</v>
       </c>
       <c r="D92" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E92" t="s" s="39">
-        <v>116</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E92" s="42"/>
     </row>
     <row r="93" ht="16" customHeight="1">
       <c r="A93" s="46"/>
       <c r="B93" s="46"/>
       <c r="C93" t="s" s="38">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D93" t="s" s="38">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="E93" s="42"/>
     </row>
@@ -4870,134 +4912,277 @@
       <c r="A94" s="46"/>
       <c r="B94" s="46"/>
       <c r="C94" t="s" s="38">
+        <v>177</v>
+      </c>
+      <c r="D94" t="s" s="38">
+        <v>178</v>
+      </c>
+      <c r="E94" s="42"/>
+    </row>
+    <row r="95" ht="16" customHeight="1">
+      <c r="A95" s="47"/>
+      <c r="B95" s="47"/>
+      <c r="C95" t="s" s="38">
         <v>179</v>
       </c>
-      <c r="D94" t="s" s="38">
-        <v>101</v>
-      </c>
-      <c r="E94" s="42"/>
-    </row>
-    <row r="95" ht="16" customHeight="1">
-      <c r="A95" s="46"/>
-      <c r="B95" s="46"/>
-      <c r="C95" t="s" s="38">
+      <c r="D95" t="s" s="38">
+        <v>149</v>
+      </c>
+      <c r="E95" s="42"/>
+    </row>
+    <row r="96" ht="16" customHeight="1">
+      <c r="A96" s="43"/>
+      <c r="B96" s="43"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="44"/>
+      <c r="E96" s="45"/>
+    </row>
+    <row r="97" ht="16" customHeight="1">
+      <c r="A97" s="36">
+        <v>16</v>
+      </c>
+      <c r="B97" t="s" s="37">
         <v>180</v>
       </c>
-      <c r="D95" t="s" s="38">
-        <v>81</v>
-      </c>
-      <c r="E95" s="42"/>
-    </row>
-    <row r="96" ht="16" customHeight="1">
-      <c r="A96" s="47"/>
-      <c r="B96" s="47"/>
-      <c r="C96" t="s" s="38">
+      <c r="C97" t="s" s="38">
+        <v>89</v>
+      </c>
+      <c r="D97" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E97" t="s" s="39">
         <v>181</v>
       </c>
-      <c r="D96" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E96" s="42"/>
-    </row>
-    <row r="97" ht="16" customHeight="1">
-      <c r="A97" s="43"/>
-      <c r="B97" s="43"/>
-      <c r="C97" s="44"/>
-      <c r="D97" s="44"/>
-      <c r="E97" s="45"/>
     </row>
     <row r="98" ht="16" customHeight="1">
-      <c r="A98" s="36">
-        <v>16</v>
-      </c>
-      <c r="B98" t="s" s="37">
-        <v>182</v>
-      </c>
+      <c r="A98" s="46"/>
+      <c r="B98" s="46"/>
       <c r="C98" t="s" s="38">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="D98" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E98" t="s" s="39">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" ht="16" customHeight="1">
       <c r="A99" s="46"/>
       <c r="B99" s="46"/>
       <c r="C99" t="s" s="38">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="D99" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E99" t="s" s="39">
-        <v>183</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E99" s="42"/>
     </row>
     <row r="100" ht="16" customHeight="1">
       <c r="A100" s="46"/>
       <c r="B100" s="46"/>
-      <c r="C100" s="48"/>
-      <c r="D100" s="48"/>
+      <c r="C100" t="s" s="38">
+        <v>183</v>
+      </c>
+      <c r="D100" t="s" s="38">
+        <v>101</v>
+      </c>
       <c r="E100" s="42"/>
     </row>
     <row r="101" ht="16" customHeight="1">
       <c r="A101" s="46"/>
       <c r="B101" s="46"/>
-      <c r="C101" s="48"/>
-      <c r="D101" s="48"/>
+      <c r="C101" t="s" s="38">
+        <v>184</v>
+      </c>
+      <c r="D101" t="s" s="38">
+        <v>81</v>
+      </c>
       <c r="E101" s="42"/>
     </row>
     <row r="102" ht="16" customHeight="1">
-      <c r="A102" s="46"/>
-      <c r="B102" s="46"/>
-      <c r="C102" s="48"/>
-      <c r="D102" s="48"/>
+      <c r="A102" s="47"/>
+      <c r="B102" s="47"/>
+      <c r="C102" t="s" s="38">
+        <v>185</v>
+      </c>
+      <c r="D102" t="s" s="38">
+        <v>90</v>
+      </c>
       <c r="E102" s="42"/>
     </row>
     <row r="103" ht="16" customHeight="1">
-      <c r="A103" s="47"/>
-      <c r="B103" s="47"/>
-      <c r="C103" s="48"/>
-      <c r="D103" s="48"/>
-      <c r="E103" s="42"/>
+      <c r="A103" s="43"/>
+      <c r="B103" s="43"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="44"/>
+      <c r="E103" s="45"/>
+    </row>
+    <row r="104" ht="16" customHeight="1">
+      <c r="A104" s="36">
+        <v>17</v>
+      </c>
+      <c r="B104" t="s" s="37">
+        <v>186</v>
+      </c>
+      <c r="C104" t="s" s="38">
+        <v>89</v>
+      </c>
+      <c r="D104" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E104" t="s" s="39">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="105" ht="16" customHeight="1">
+      <c r="A105" s="46"/>
+      <c r="B105" s="46"/>
+      <c r="C105" t="s" s="38">
+        <v>157</v>
+      </c>
+      <c r="D105" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E105" t="s" s="39">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="106" ht="16" customHeight="1">
+      <c r="A106" s="46"/>
+      <c r="B106" s="46"/>
+      <c r="C106" s="50"/>
+      <c r="D106" s="50"/>
+      <c r="E106" s="42"/>
+    </row>
+    <row r="107" ht="16" customHeight="1">
+      <c r="A107" s="46"/>
+      <c r="B107" s="46"/>
+      <c r="C107" s="50"/>
+      <c r="D107" s="50"/>
+      <c r="E107" s="42"/>
+    </row>
+    <row r="108" ht="16" customHeight="1">
+      <c r="A108" s="46"/>
+      <c r="B108" s="46"/>
+      <c r="C108" s="50"/>
+      <c r="D108" s="50"/>
+      <c r="E108" s="42"/>
+    </row>
+    <row r="109" ht="16" customHeight="1">
+      <c r="A109" s="47"/>
+      <c r="B109" s="47"/>
+      <c r="C109" s="50"/>
+      <c r="D109" s="50"/>
+      <c r="E109" s="42"/>
+    </row>
+    <row r="110" ht="16" customHeight="1">
+      <c r="A110" s="43"/>
+      <c r="B110" s="43"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="44"/>
+      <c r="E110" s="45"/>
+    </row>
+    <row r="111" ht="16" customHeight="1">
+      <c r="A111" s="36">
+        <v>18</v>
+      </c>
+      <c r="B111" t="s" s="37">
+        <v>188</v>
+      </c>
+      <c r="C111" t="s" s="38">
+        <v>139</v>
+      </c>
+      <c r="D111" t="s" s="38">
+        <v>81</v>
+      </c>
+      <c r="E111" t="s" s="39">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="112" ht="16" customHeight="1">
+      <c r="A112" s="40"/>
+      <c r="B112" s="40"/>
+      <c r="C112" t="s" s="38">
+        <v>188</v>
+      </c>
+      <c r="D112" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="E112" t="s" s="39">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" ht="16" customHeight="1">
+      <c r="A113" s="40"/>
+      <c r="B113" s="40"/>
+      <c r="C113" t="s" s="38">
+        <v>189</v>
+      </c>
+      <c r="D113" t="s" s="38">
+        <v>87</v>
+      </c>
+      <c r="E113" s="42"/>
+    </row>
+    <row r="114" ht="16" customHeight="1">
+      <c r="A114" s="40"/>
+      <c r="B114" s="40"/>
+      <c r="C114" s="50"/>
+      <c r="D114" s="50"/>
+      <c r="E114" s="42"/>
+    </row>
+    <row r="115" ht="16" customHeight="1">
+      <c r="A115" s="40"/>
+      <c r="B115" s="40"/>
+      <c r="C115" s="50"/>
+      <c r="D115" s="50"/>
+      <c r="E115" s="42"/>
+    </row>
+    <row r="116" ht="16" customHeight="1">
+      <c r="A116" s="41"/>
+      <c r="B116" s="41"/>
+      <c r="C116" s="50"/>
+      <c r="D116" s="50"/>
+      <c r="E116" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="B91:B96"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="B81:B89"/>
-    <mergeCell ref="A81:A89"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="A64:A75"/>
-    <mergeCell ref="B77:B79"/>
+  <mergeCells count="36">
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B70:B81"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="B33:B41"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="A49:A51"/>
     <mergeCell ref="B59:B62"/>
+    <mergeCell ref="A53:A57"/>
     <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="B98:B103"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B29:B37"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B64:B75"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B97:B102"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="B104:B109"/>
+    <mergeCell ref="A70:A81"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A87:A95"/>
+    <mergeCell ref="B87:B95"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="B111:B116"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Updates for test cases and schema documentation
</commit_message>
<xml_diff>
--- a/documents/QMe_UserStories.xlsx
+++ b/documents/QMe_UserStories.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="191">
   <si>
     <t>Project</t>
   </si>
@@ -411,6 +411,9 @@
   </si>
   <si>
     <t>QUESTION_UPDATE_USER</t>
+  </si>
+  <si>
+    <t>QUESTION_POINT</t>
   </si>
   <si>
     <t>QUESTION_HIT</t>
@@ -927,7 +930,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1077,6 +1080,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
@@ -1321,10 +1330,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>374191</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>21118</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>480099</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95447</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1341,8 +1350,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-1" y="0"/>
-          <a:ext cx="7867193" cy="9501669"/>
+          <a:off x="-125750" y="-364064"/>
+          <a:ext cx="7363500" cy="8766374"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2699,10 +2708,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B3:F11"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B2:F2"/>
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B3:F11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
@@ -3795,7 +3804,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -4297,58 +4306,58 @@
       </c>
     </row>
     <row r="42" ht="16" customHeight="1">
-      <c r="A42" s="43"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="51"/>
+      <c r="C42" t="s" s="38">
+        <v>131</v>
+      </c>
+      <c r="D42" t="s" s="38">
+        <v>81</v>
+      </c>
+      <c r="E42" s="49"/>
     </row>
     <row r="43" ht="16" customHeight="1">
-      <c r="A43" s="36">
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="45"/>
+    </row>
+    <row r="44" ht="16" customHeight="1">
+      <c r="A44" s="36">
         <v>8</v>
       </c>
-      <c r="B43" t="s" s="37">
-        <v>131</v>
-      </c>
-      <c r="C43" t="s" s="38">
+      <c r="B44" t="s" s="37">
+        <v>132</v>
+      </c>
+      <c r="C44" t="s" s="38">
         <v>121</v>
-      </c>
-      <c r="D43" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E43" t="s" s="39">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" ht="16" customHeight="1">
-      <c r="A44" s="46"/>
-      <c r="B44" s="46"/>
-      <c r="C44" t="s" s="38">
-        <v>108</v>
       </c>
       <c r="D44" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E44" t="s" s="39">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" ht="16" customHeight="1">
       <c r="A45" s="46"/>
       <c r="B45" s="46"/>
       <c r="C45" t="s" s="38">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="D45" t="s" s="38">
-        <v>81</v>
-      </c>
-      <c r="E45" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E45" t="s" s="39">
+        <v>116</v>
+      </c>
     </row>
     <row r="46" ht="16" customHeight="1">
       <c r="A46" s="46"/>
       <c r="B46" s="46"/>
       <c r="C46" t="s" s="38">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D46" t="s" s="38">
         <v>81</v>
@@ -4356,8 +4365,8 @@
       <c r="E46" s="42"/>
     </row>
     <row r="47" ht="16" customHeight="1">
-      <c r="A47" s="47"/>
-      <c r="B47" s="47"/>
+      <c r="A47" s="46"/>
+      <c r="B47" s="46"/>
       <c r="C47" t="s" s="38">
         <v>134</v>
       </c>
@@ -4367,297 +4376,297 @@
       <c r="E47" s="42"/>
     </row>
     <row r="48" ht="16" customHeight="1">
-      <c r="A48" s="43"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="45"/>
+      <c r="A48" s="47"/>
+      <c r="B48" s="47"/>
+      <c r="C48" t="s" s="38">
+        <v>135</v>
+      </c>
+      <c r="D48" t="s" s="38">
+        <v>81</v>
+      </c>
+      <c r="E48" s="42"/>
     </row>
     <row r="49" ht="16" customHeight="1">
-      <c r="A49" s="36">
+      <c r="A49" s="43"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="45"/>
+    </row>
+    <row r="50" ht="16" customHeight="1">
+      <c r="A50" s="36">
         <v>9</v>
       </c>
-      <c r="B49" t="s" s="37">
-        <v>135</v>
-      </c>
-      <c r="C49" t="s" s="38">
+      <c r="B50" t="s" s="37">
+        <v>136</v>
+      </c>
+      <c r="C50" t="s" s="38">
         <v>89</v>
-      </c>
-      <c r="D49" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E49" t="s" s="39">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="50" ht="16" customHeight="1">
-      <c r="A50" s="46"/>
-      <c r="B50" s="46"/>
-      <c r="C50" t="s" s="38">
-        <v>121</v>
       </c>
       <c r="D50" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E50" t="s" s="39">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" ht="16" customHeight="1">
-      <c r="A51" s="47"/>
-      <c r="B51" s="47"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="42"/>
+      <c r="A51" s="46"/>
+      <c r="B51" s="46"/>
+      <c r="C51" t="s" s="38">
+        <v>121</v>
+      </c>
+      <c r="D51" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E51" t="s" s="39">
+        <v>133</v>
+      </c>
     </row>
     <row r="52" ht="16" customHeight="1">
-      <c r="A52" s="43"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="45"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="42"/>
     </row>
     <row r="53" ht="16" customHeight="1">
-      <c r="A53" s="36">
+      <c r="A53" s="43"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="45"/>
+    </row>
+    <row r="54" ht="16" customHeight="1">
+      <c r="A54" s="36">
         <v>10</v>
       </c>
-      <c r="B53" t="s" s="37">
-        <v>137</v>
-      </c>
-      <c r="C53" t="s" s="38">
+      <c r="B54" t="s" s="37">
         <v>138</v>
       </c>
-      <c r="D53" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E53" t="s" s="39">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" ht="16" customHeight="1">
-      <c r="A54" s="46"/>
-      <c r="B54" s="46"/>
       <c r="C54" t="s" s="38">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="D54" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E54" t="s" s="39">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" ht="16" customHeight="1">
       <c r="A55" s="46"/>
       <c r="B55" s="46"/>
       <c r="C55" t="s" s="38">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="D55" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E55" t="s" s="39">
         <v>81</v>
       </c>
-      <c r="E55" t="s" s="39">
+    </row>
+    <row r="56" ht="16" customHeight="1">
+      <c r="A56" s="46"/>
+      <c r="B56" s="46"/>
+      <c r="C56" t="s" s="38">
         <v>140</v>
       </c>
-    </row>
-    <row r="56" ht="16" customHeight="1">
-      <c r="A56" s="31"/>
-      <c r="B56" s="51"/>
-      <c r="C56" t="s" s="38">
+      <c r="D56" t="s" s="38">
+        <v>81</v>
+      </c>
+      <c r="E56" t="s" s="39">
         <v>141</v>
       </c>
-      <c r="D56" t="s" s="38">
-        <v>110</v>
-      </c>
-      <c r="E56" s="42"/>
     </row>
     <row r="57" ht="16" customHeight="1">
-      <c r="A57" s="47"/>
-      <c r="B57" s="47"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="53"/>
       <c r="C57" t="s" s="38">
         <v>142</v>
       </c>
       <c r="D57" t="s" s="38">
+        <v>110</v>
+      </c>
+      <c r="E57" s="42"/>
+    </row>
+    <row r="58" ht="16" customHeight="1">
+      <c r="A58" s="47"/>
+      <c r="B58" s="47"/>
+      <c r="C58" t="s" s="38">
         <v>143</v>
       </c>
-      <c r="E57" s="42"/>
-    </row>
-    <row r="58" ht="16" customHeight="1">
-      <c r="A58" s="43"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="45"/>
+      <c r="D58" t="s" s="38">
+        <v>144</v>
+      </c>
+      <c r="E58" s="42"/>
     </row>
     <row r="59" ht="16" customHeight="1">
-      <c r="A59" s="36">
+      <c r="A59" s="43"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="45"/>
+    </row>
+    <row r="60" ht="16" customHeight="1">
+      <c r="A60" s="36">
         <v>11</v>
       </c>
-      <c r="B59" t="s" s="37">
-        <v>144</v>
-      </c>
-      <c r="C59" t="s" s="38">
+      <c r="B60" t="s" s="37">
         <v>145</v>
       </c>
-      <c r="D59" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E59" t="s" s="39">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" ht="16" customHeight="1">
-      <c r="A60" s="46"/>
-      <c r="B60" s="46"/>
       <c r="C60" t="s" s="38">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="D60" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E60" t="s" s="39">
-        <v>146</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" ht="16" customHeight="1">
       <c r="A61" s="46"/>
       <c r="B61" s="46"/>
       <c r="C61" t="s" s="38">
+        <v>121</v>
+      </c>
+      <c r="D61" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E61" t="s" s="39">
         <v>147</v>
       </c>
-      <c r="D61" t="s" s="38">
-        <v>123</v>
-      </c>
-      <c r="E61" s="42"/>
     </row>
     <row r="62" ht="16" customHeight="1">
-      <c r="A62" s="47"/>
-      <c r="B62" s="47"/>
+      <c r="A62" s="46"/>
+      <c r="B62" s="46"/>
       <c r="C62" t="s" s="38">
         <v>148</v>
       </c>
       <c r="D62" t="s" s="38">
+        <v>123</v>
+      </c>
+      <c r="E62" s="42"/>
+    </row>
+    <row r="63" ht="16" customHeight="1">
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
+      <c r="C63" t="s" s="38">
         <v>149</v>
       </c>
-      <c r="E62" t="s" s="39">
+      <c r="D63" t="s" s="38">
         <v>150</v>
       </c>
-    </row>
-    <row r="63" ht="16" customHeight="1">
-      <c r="A63" s="43"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="45"/>
+      <c r="E63" t="s" s="39">
+        <v>151</v>
+      </c>
     </row>
     <row r="64" ht="16" customHeight="1">
-      <c r="A64" s="36">
+      <c r="A64" s="43"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="45"/>
+    </row>
+    <row r="65" ht="16" customHeight="1">
+      <c r="A65" s="36">
         <v>12</v>
       </c>
-      <c r="B64" t="s" s="37">
-        <v>151</v>
-      </c>
-      <c r="C64" t="s" s="38">
+      <c r="B65" t="s" s="37">
         <v>152</v>
       </c>
-      <c r="D64" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E64" t="s" s="39">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" ht="16" customHeight="1">
-      <c r="A65" s="46"/>
-      <c r="B65" s="46"/>
       <c r="C65" t="s" s="38">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D65" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E65" t="s" s="39">
-        <v>153</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" ht="16" customHeight="1">
       <c r="A66" s="46"/>
       <c r="B66" s="46"/>
       <c r="C66" t="s" s="38">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D66" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E66" t="s" s="39">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" ht="16" customHeight="1">
+      <c r="A67" s="46"/>
+      <c r="B67" s="46"/>
+      <c r="C67" t="s" s="38">
+        <v>140</v>
+      </c>
+      <c r="D67" t="s" s="38">
         <v>81</v>
       </c>
-      <c r="E66" t="s" s="39">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="67" ht="16" customHeight="1">
-      <c r="A67" s="31"/>
-      <c r="B67" s="51"/>
-      <c r="C67" t="s" s="38">
-        <v>154</v>
-      </c>
-      <c r="D67" t="s" s="38">
-        <v>110</v>
-      </c>
-      <c r="E67" s="42"/>
+      <c r="E67" t="s" s="39">
+        <v>141</v>
+      </c>
     </row>
     <row r="68" ht="16" customHeight="1">
-      <c r="A68" s="47"/>
-      <c r="B68" s="47"/>
+      <c r="A68" s="31"/>
+      <c r="B68" s="53"/>
       <c r="C68" t="s" s="38">
         <v>155</v>
       </c>
       <c r="D68" t="s" s="38">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="E68" s="42"/>
     </row>
     <row r="69" ht="16" customHeight="1">
-      <c r="A69" s="43"/>
-      <c r="B69" s="43"/>
-      <c r="C69" s="44"/>
-      <c r="D69" s="44"/>
-      <c r="E69" s="45"/>
+      <c r="A69" s="47"/>
+      <c r="B69" s="47"/>
+      <c r="C69" t="s" s="38">
+        <v>156</v>
+      </c>
+      <c r="D69" t="s" s="38">
+        <v>144</v>
+      </c>
+      <c r="E69" s="42"/>
     </row>
     <row r="70" ht="16" customHeight="1">
-      <c r="A70" s="36">
+      <c r="A70" s="43"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="45"/>
+    </row>
+    <row r="71" ht="16" customHeight="1">
+      <c r="A71" s="36">
         <v>13</v>
       </c>
-      <c r="B70" t="s" s="37">
-        <v>156</v>
-      </c>
-      <c r="C70" t="s" s="38">
+      <c r="B71" t="s" s="37">
         <v>157</v>
       </c>
-      <c r="D70" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E70" t="s" s="39">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="71" ht="16" customHeight="1">
-      <c r="A71" s="46"/>
-      <c r="B71" s="46"/>
       <c r="C71" t="s" s="38">
         <v>158</v>
       </c>
       <c r="D71" t="s" s="38">
-        <v>159</v>
-      </c>
-      <c r="E71" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E71" t="s" s="39">
+        <v>82</v>
+      </c>
     </row>
     <row r="72" ht="16" customHeight="1">
       <c r="A72" s="46"/>
       <c r="B72" s="46"/>
       <c r="C72" t="s" s="38">
+        <v>159</v>
+      </c>
+      <c r="D72" t="s" s="38">
         <v>160</v>
-      </c>
-      <c r="D72" t="s" s="38">
-        <v>161</v>
       </c>
       <c r="E72" s="42"/>
     </row>
@@ -4665,25 +4674,25 @@
       <c r="A73" s="46"/>
       <c r="B73" s="46"/>
       <c r="C73" t="s" s="38">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="D73" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E73" t="s" s="39">
-        <v>116</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="E73" s="42"/>
     </row>
     <row r="74" ht="16" customHeight="1">
       <c r="A74" s="46"/>
       <c r="B74" s="46"/>
       <c r="C74" t="s" s="38">
-        <v>162</v>
+        <v>108</v>
       </c>
       <c r="D74" t="s" s="38">
         <v>90</v>
       </c>
-      <c r="E74" s="42"/>
+      <c r="E74" t="s" s="39">
+        <v>116</v>
+      </c>
     </row>
     <row r="75" ht="16" customHeight="1">
       <c r="A75" s="46"/>
@@ -4703,7 +4712,7 @@
         <v>164</v>
       </c>
       <c r="D76" t="s" s="38">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="E76" s="42"/>
     </row>
@@ -4714,7 +4723,7 @@
         <v>165</v>
       </c>
       <c r="D77" t="s" s="38">
-        <v>101</v>
+        <v>150</v>
       </c>
       <c r="E77" s="42"/>
     </row>
@@ -4725,11 +4734,9 @@
         <v>166</v>
       </c>
       <c r="D78" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E78" t="s" s="39">
-        <v>105</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E78" s="42"/>
     </row>
     <row r="79" ht="16" customHeight="1">
       <c r="A79" s="46"/>
@@ -4738,9 +4745,11 @@
         <v>167</v>
       </c>
       <c r="D79" t="s" s="38">
-        <v>101</v>
-      </c>
-      <c r="E79" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E79" t="s" s="39">
+        <v>105</v>
+      </c>
     </row>
     <row r="80" ht="16" customHeight="1">
       <c r="A80" s="46"/>
@@ -4749,142 +4758,142 @@
         <v>168</v>
       </c>
       <c r="D80" t="s" s="38">
+        <v>101</v>
+      </c>
+      <c r="E80" s="42"/>
+    </row>
+    <row r="81" ht="16" customHeight="1">
+      <c r="A81" s="46"/>
+      <c r="B81" s="46"/>
+      <c r="C81" t="s" s="38">
+        <v>169</v>
+      </c>
+      <c r="D81" t="s" s="38">
         <v>90</v>
       </c>
-      <c r="E80" t="s" s="39">
+      <c r="E81" t="s" s="39">
         <v>105</v>
       </c>
     </row>
-    <row r="81" ht="16" customHeight="1">
-      <c r="A81" s="47"/>
-      <c r="B81" s="47"/>
-      <c r="C81" s="52"/>
-      <c r="D81" s="52"/>
-      <c r="E81" s="53"/>
-    </row>
     <row r="82" ht="16" customHeight="1">
-      <c r="A82" s="43"/>
-      <c r="B82" s="43"/>
-      <c r="C82" s="44"/>
-      <c r="D82" s="44"/>
-      <c r="E82" s="45"/>
+      <c r="A82" s="47"/>
+      <c r="B82" s="47"/>
+      <c r="C82" s="54"/>
+      <c r="D82" s="54"/>
+      <c r="E82" s="55"/>
     </row>
     <row r="83" ht="16" customHeight="1">
-      <c r="A83" s="36">
+      <c r="A83" s="43"/>
+      <c r="B83" s="43"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="45"/>
+    </row>
+    <row r="84" ht="16" customHeight="1">
+      <c r="A84" s="36">
         <v>14</v>
       </c>
-      <c r="B83" t="s" s="37">
-        <v>169</v>
-      </c>
-      <c r="C83" t="s" s="38">
+      <c r="B84" t="s" s="37">
         <v>170</v>
       </c>
-      <c r="D83" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E83" t="s" s="39">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" ht="16" customHeight="1">
-      <c r="A84" s="46"/>
-      <c r="B84" s="46"/>
       <c r="C84" t="s" s="38">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="D84" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E84" t="s" s="39">
-        <v>171</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" ht="16" customHeight="1">
-      <c r="A85" s="47"/>
-      <c r="B85" s="47"/>
+      <c r="A85" s="46"/>
+      <c r="B85" s="46"/>
       <c r="C85" t="s" s="38">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="D85" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E85" t="s" s="39">
-        <v>146</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" ht="16" customHeight="1">
-      <c r="A86" s="43"/>
-      <c r="B86" s="43"/>
-      <c r="C86" s="44"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="45"/>
+      <c r="A86" s="47"/>
+      <c r="B86" s="47"/>
+      <c r="C86" t="s" s="38">
+        <v>121</v>
+      </c>
+      <c r="D86" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E86" t="s" s="39">
+        <v>147</v>
+      </c>
     </row>
     <row r="87" ht="16" customHeight="1">
-      <c r="A87" s="36">
+      <c r="A87" s="43"/>
+      <c r="B87" s="43"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="45"/>
+    </row>
+    <row r="88" ht="16" customHeight="1">
+      <c r="A88" s="36">
         <v>15</v>
       </c>
-      <c r="B87" t="s" s="37">
-        <v>172</v>
-      </c>
-      <c r="C87" t="s" s="38">
+      <c r="B88" t="s" s="37">
         <v>173</v>
       </c>
-      <c r="D87" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E87" t="s" s="39">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="88" ht="16" customHeight="1">
-      <c r="A88" s="46"/>
-      <c r="B88" s="46"/>
       <c r="C88" t="s" s="38">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="D88" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E88" t="s" s="39">
-        <v>105</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89" ht="16" customHeight="1">
       <c r="A89" s="46"/>
       <c r="B89" s="46"/>
       <c r="C89" t="s" s="38">
-        <v>157</v>
+        <v>89</v>
       </c>
       <c r="D89" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E89" t="s" s="39">
-        <v>171</v>
+        <v>105</v>
       </c>
     </row>
     <row r="90" ht="16" customHeight="1">
       <c r="A90" s="46"/>
       <c r="B90" s="46"/>
       <c r="C90" t="s" s="38">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="D90" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E90" t="s" s="39">
-        <v>116</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" ht="16" customHeight="1">
       <c r="A91" s="46"/>
       <c r="B91" s="46"/>
       <c r="C91" t="s" s="38">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="D91" t="s" s="38">
-        <v>101</v>
-      </c>
-      <c r="E91" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E91" t="s" s="39">
+        <v>116</v>
+      </c>
     </row>
     <row r="92" ht="16" customHeight="1">
       <c r="A92" s="46"/>
@@ -4904,7 +4913,7 @@
         <v>176</v>
       </c>
       <c r="D93" t="s" s="38">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E93" s="42"/>
     </row>
@@ -4915,68 +4924,68 @@
         <v>177</v>
       </c>
       <c r="D94" t="s" s="38">
+        <v>81</v>
+      </c>
+      <c r="E94" s="42"/>
+    </row>
+    <row r="95" ht="16" customHeight="1">
+      <c r="A95" s="46"/>
+      <c r="B95" s="46"/>
+      <c r="C95" t="s" s="38">
         <v>178</v>
       </c>
-      <c r="E94" s="42"/>
-    </row>
-    <row r="95" ht="16" customHeight="1">
-      <c r="A95" s="47"/>
-      <c r="B95" s="47"/>
-      <c r="C95" t="s" s="38">
+      <c r="D95" t="s" s="38">
         <v>179</v>
       </c>
-      <c r="D95" t="s" s="38">
-        <v>149</v>
-      </c>
       <c r="E95" s="42"/>
     </row>
     <row r="96" ht="16" customHeight="1">
-      <c r="A96" s="43"/>
-      <c r="B96" s="43"/>
-      <c r="C96" s="44"/>
-      <c r="D96" s="44"/>
-      <c r="E96" s="45"/>
+      <c r="A96" s="47"/>
+      <c r="B96" s="47"/>
+      <c r="C96" t="s" s="38">
+        <v>180</v>
+      </c>
+      <c r="D96" t="s" s="38">
+        <v>150</v>
+      </c>
+      <c r="E96" s="42"/>
     </row>
     <row r="97" ht="16" customHeight="1">
-      <c r="A97" s="36">
+      <c r="A97" s="43"/>
+      <c r="B97" s="43"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="44"/>
+      <c r="E97" s="45"/>
+    </row>
+    <row r="98" ht="16" customHeight="1">
+      <c r="A98" s="36">
         <v>16</v>
       </c>
-      <c r="B97" t="s" s="37">
-        <v>180</v>
-      </c>
-      <c r="C97" t="s" s="38">
+      <c r="B98" t="s" s="37">
+        <v>181</v>
+      </c>
+      <c r="C98" t="s" s="38">
         <v>89</v>
-      </c>
-      <c r="D97" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E97" t="s" s="39">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="98" ht="16" customHeight="1">
-      <c r="A98" s="46"/>
-      <c r="B98" s="46"/>
-      <c r="C98" t="s" s="38">
-        <v>108</v>
       </c>
       <c r="D98" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E98" t="s" s="39">
-        <v>116</v>
+        <v>182</v>
       </c>
     </row>
     <row r="99" ht="16" customHeight="1">
       <c r="A99" s="46"/>
       <c r="B99" s="46"/>
       <c r="C99" t="s" s="38">
-        <v>182</v>
+        <v>108</v>
       </c>
       <c r="D99" t="s" s="38">
-        <v>101</v>
-      </c>
-      <c r="E99" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="E99" t="s" s="39">
+        <v>116</v>
+      </c>
     </row>
     <row r="100" ht="16" customHeight="1">
       <c r="A100" s="46"/>
@@ -4996,121 +5005,119 @@
         <v>184</v>
       </c>
       <c r="D101" t="s" s="38">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E101" s="42"/>
     </row>
     <row r="102" ht="16" customHeight="1">
-      <c r="A102" s="47"/>
-      <c r="B102" s="47"/>
+      <c r="A102" s="46"/>
+      <c r="B102" s="46"/>
       <c r="C102" t="s" s="38">
         <v>185</v>
       </c>
       <c r="D102" t="s" s="38">
+        <v>81</v>
+      </c>
+      <c r="E102" s="42"/>
+    </row>
+    <row r="103" ht="16" customHeight="1">
+      <c r="A103" s="47"/>
+      <c r="B103" s="47"/>
+      <c r="C103" t="s" s="38">
+        <v>186</v>
+      </c>
+      <c r="D103" t="s" s="38">
         <v>90</v>
       </c>
-      <c r="E102" s="42"/>
-    </row>
-    <row r="103" ht="16" customHeight="1">
-      <c r="A103" s="43"/>
-      <c r="B103" s="43"/>
-      <c r="C103" s="44"/>
-      <c r="D103" s="44"/>
-      <c r="E103" s="45"/>
+      <c r="E103" s="42"/>
     </row>
     <row r="104" ht="16" customHeight="1">
-      <c r="A104" s="36">
+      <c r="A104" s="43"/>
+      <c r="B104" s="43"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="45"/>
+    </row>
+    <row r="105" ht="16" customHeight="1">
+      <c r="A105" s="36">
         <v>17</v>
       </c>
-      <c r="B104" t="s" s="37">
-        <v>186</v>
-      </c>
-      <c r="C104" t="s" s="38">
+      <c r="B105" t="s" s="37">
+        <v>187</v>
+      </c>
+      <c r="C105" t="s" s="38">
         <v>89</v>
-      </c>
-      <c r="D104" t="s" s="38">
-        <v>90</v>
-      </c>
-      <c r="E104" t="s" s="39">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="105" ht="16" customHeight="1">
-      <c r="A105" s="46"/>
-      <c r="B105" s="46"/>
-      <c r="C105" t="s" s="38">
-        <v>157</v>
       </c>
       <c r="D105" t="s" s="38">
         <v>90</v>
       </c>
       <c r="E105" t="s" s="39">
-        <v>187</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" ht="16" customHeight="1">
       <c r="A106" s="46"/>
       <c r="B106" s="46"/>
-      <c r="C106" s="50"/>
-      <c r="D106" s="50"/>
-      <c r="E106" s="42"/>
+      <c r="C106" t="s" s="38">
+        <v>158</v>
+      </c>
+      <c r="D106" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E106" t="s" s="39">
+        <v>188</v>
+      </c>
     </row>
     <row r="107" ht="16" customHeight="1">
       <c r="A107" s="46"/>
       <c r="B107" s="46"/>
-      <c r="C107" s="50"/>
-      <c r="D107" s="50"/>
+      <c r="C107" s="52"/>
+      <c r="D107" s="52"/>
       <c r="E107" s="42"/>
     </row>
     <row r="108" ht="16" customHeight="1">
       <c r="A108" s="46"/>
       <c r="B108" s="46"/>
-      <c r="C108" s="50"/>
-      <c r="D108" s="50"/>
+      <c r="C108" s="52"/>
+      <c r="D108" s="52"/>
       <c r="E108" s="42"/>
     </row>
     <row r="109" ht="16" customHeight="1">
-      <c r="A109" s="47"/>
-      <c r="B109" s="47"/>
-      <c r="C109" s="50"/>
-      <c r="D109" s="50"/>
+      <c r="A109" s="46"/>
+      <c r="B109" s="46"/>
+      <c r="C109" s="52"/>
+      <c r="D109" s="52"/>
       <c r="E109" s="42"/>
     </row>
     <row r="110" ht="16" customHeight="1">
-      <c r="A110" s="43"/>
-      <c r="B110" s="43"/>
-      <c r="C110" s="44"/>
-      <c r="D110" s="44"/>
-      <c r="E110" s="45"/>
+      <c r="A110" s="47"/>
+      <c r="B110" s="47"/>
+      <c r="C110" s="52"/>
+      <c r="D110" s="52"/>
+      <c r="E110" s="42"/>
     </row>
     <row r="111" ht="16" customHeight="1">
-      <c r="A111" s="36">
+      <c r="A111" s="43"/>
+      <c r="B111" s="43"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="44"/>
+      <c r="E111" s="45"/>
+    </row>
+    <row r="112" ht="16" customHeight="1">
+      <c r="A112" s="36">
         <v>18</v>
       </c>
-      <c r="B111" t="s" s="37">
-        <v>188</v>
-      </c>
-      <c r="C111" t="s" s="38">
-        <v>139</v>
-      </c>
-      <c r="D111" t="s" s="38">
+      <c r="B112" t="s" s="37">
+        <v>189</v>
+      </c>
+      <c r="C112" t="s" s="38">
+        <v>140</v>
+      </c>
+      <c r="D112" t="s" s="38">
         <v>81</v>
       </c>
-      <c r="E111" t="s" s="39">
+      <c r="E112" t="s" s="39">
         <v>82</v>
-      </c>
-    </row>
-    <row r="112" ht="16" customHeight="1">
-      <c r="A112" s="40"/>
-      <c r="B112" s="40"/>
-      <c r="C112" t="s" s="38">
-        <v>188</v>
-      </c>
-      <c r="D112" t="s" s="38">
-        <v>84</v>
-      </c>
-      <c r="E112" t="s" s="39">
-        <v>85</v>
       </c>
     </row>
     <row r="113" ht="16" customHeight="1">
@@ -5120,69 +5127,82 @@
         <v>189</v>
       </c>
       <c r="D113" t="s" s="38">
-        <v>87</v>
-      </c>
-      <c r="E113" s="42"/>
+        <v>84</v>
+      </c>
+      <c r="E113" t="s" s="39">
+        <v>85</v>
+      </c>
     </row>
     <row r="114" ht="16" customHeight="1">
       <c r="A114" s="40"/>
       <c r="B114" s="40"/>
-      <c r="C114" s="50"/>
-      <c r="D114" s="50"/>
+      <c r="C114" t="s" s="38">
+        <v>190</v>
+      </c>
+      <c r="D114" t="s" s="38">
+        <v>87</v>
+      </c>
       <c r="E114" s="42"/>
     </row>
     <row r="115" ht="16" customHeight="1">
       <c r="A115" s="40"/>
       <c r="B115" s="40"/>
-      <c r="C115" s="50"/>
-      <c r="D115" s="50"/>
+      <c r="C115" s="52"/>
+      <c r="D115" s="52"/>
       <c r="E115" s="42"/>
     </row>
     <row r="116" ht="16" customHeight="1">
-      <c r="A116" s="41"/>
-      <c r="B116" s="41"/>
-      <c r="C116" s="50"/>
-      <c r="D116" s="50"/>
+      <c r="A116" s="40"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="52"/>
+      <c r="D116" s="52"/>
       <c r="E116" s="42"/>
+    </row>
+    <row r="117" ht="16" customHeight="1">
+      <c r="A117" s="41"/>
+      <c r="B117" s="41"/>
+      <c r="C117" s="52"/>
+      <c r="D117" s="52"/>
+      <c r="E117" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B33:B41"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B50:B52"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B70:B81"/>
-    <mergeCell ref="A33:A41"/>
-    <mergeCell ref="B33:B41"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B97:B102"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="B104:B109"/>
-    <mergeCell ref="A70:A81"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A87:A95"/>
-    <mergeCell ref="B87:B95"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="B111:B116"/>
+    <mergeCell ref="B112:B117"/>
+    <mergeCell ref="A112:A117"/>
+    <mergeCell ref="A105:A110"/>
+    <mergeCell ref="A98:A103"/>
+    <mergeCell ref="B88:B96"/>
+    <mergeCell ref="A88:A96"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A71:A82"/>
+    <mergeCell ref="B105:B110"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B98:B103"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B71:B82"/>
+    <mergeCell ref="B65:B69"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
updates to add password reset schema
</commit_message>
<xml_diff>
--- a/documents/QMe_UserStories.xlsx
+++ b/documents/QMe_UserStories.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="194">
   <si>
     <t>Project</t>
   </si>
@@ -591,6 +591,15 @@
   </si>
   <si>
     <t>MEDIA_TYPE_DESC</t>
+  </si>
+  <si>
+    <t>USER_PASSWORD_RESET</t>
+  </si>
+  <si>
+    <t>RESET_TOKEN</t>
+  </si>
+  <si>
+    <t>CREATED_TIMESTAMP</t>
   </si>
 </sst>
 </file>
@@ -1330,10 +1339,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>480099</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>95447</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>46373</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>100145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1350,8 +1359,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-125750" y="-364064"/>
-          <a:ext cx="7363500" cy="8766374"/>
+          <a:off x="-119380" y="-279400"/>
+          <a:ext cx="8148974" cy="7961446"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2708,10 +2717,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="A3:A11"/>
     <mergeCell ref="B3:F11"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
@@ -3804,7 +3813,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -5165,44 +5174,113 @@
       <c r="D117" s="52"/>
       <c r="E117" s="42"/>
     </row>
+    <row r="118" ht="16" customHeight="1">
+      <c r="A118" s="43"/>
+      <c r="B118" s="43"/>
+      <c r="C118" s="44"/>
+      <c r="D118" s="44"/>
+      <c r="E118" s="45"/>
+    </row>
+    <row r="119" ht="16" customHeight="1">
+      <c r="A119" s="36">
+        <v>19</v>
+      </c>
+      <c r="B119" t="s" s="37">
+        <v>191</v>
+      </c>
+      <c r="C119" t="s" s="38">
+        <v>89</v>
+      </c>
+      <c r="D119" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E119" t="s" s="39">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="120" ht="16" customHeight="1">
+      <c r="A120" s="40"/>
+      <c r="B120" s="40"/>
+      <c r="C120" t="s" s="38">
+        <v>192</v>
+      </c>
+      <c r="D120" t="s" s="38">
+        <v>90</v>
+      </c>
+      <c r="E120" s="42"/>
+    </row>
+    <row r="121" ht="16" customHeight="1">
+      <c r="A121" s="40"/>
+      <c r="B121" s="40"/>
+      <c r="C121" t="s" s="38">
+        <v>193</v>
+      </c>
+      <c r="D121" t="s" s="38">
+        <v>101</v>
+      </c>
+      <c r="E121" s="42"/>
+    </row>
+    <row r="122" ht="16" customHeight="1">
+      <c r="A122" s="40"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="52"/>
+      <c r="D122" s="52"/>
+      <c r="E122" s="42"/>
+    </row>
+    <row r="123" ht="16" customHeight="1">
+      <c r="A123" s="40"/>
+      <c r="B123" s="40"/>
+      <c r="C123" s="52"/>
+      <c r="D123" s="52"/>
+      <c r="E123" s="42"/>
+    </row>
+    <row r="124" ht="16" customHeight="1">
+      <c r="A124" s="41"/>
+      <c r="B124" s="41"/>
+      <c r="C124" s="52"/>
+      <c r="D124" s="52"/>
+      <c r="E124" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="38">
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="B71:B82"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="B98:B103"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B105:B110"/>
+    <mergeCell ref="A71:A82"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A88:A96"/>
+    <mergeCell ref="B88:B96"/>
+    <mergeCell ref="A98:A103"/>
+    <mergeCell ref="A105:A110"/>
+    <mergeCell ref="A112:A117"/>
+    <mergeCell ref="B112:B117"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A33:A41"/>
     <mergeCell ref="B33:B41"/>
-    <mergeCell ref="A33:A41"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B112:B117"/>
-    <mergeCell ref="A112:A117"/>
-    <mergeCell ref="A105:A110"/>
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="B88:B96"/>
-    <mergeCell ref="A88:A96"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="A71:A82"/>
-    <mergeCell ref="B105:B110"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B98:B103"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="B71:B82"/>
-    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="B119:B124"/>
+    <mergeCell ref="A119:A124"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>